<commit_message>
DGT archetypes and USE_TYPE_PROPERTIES
</commit_message>
<xml_diff>
--- a/remap_ville_plugin/CH_ReMaP/archetypes/SURB_2040_DGT/use_types/USE_TYPE_PROPERTIES.xlsx
+++ b/remap_ville_plugin/CH_ReMaP/archetypes/SURB_2040_DGT/use_types/USE_TYPE_PROPERTIES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shsieh\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\CH_ReMaP\archetypes\SURB_2040_DGT\use_types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\03-Research\01-Projects\30_VILLE\CEA_Projects\_CaseStudies\Echallens\CEA_simulations\2060_DGT_RCP85\inputs\technology\archetypes\use_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23155A5-0A35-4175-B8C9-85CB994779C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3406187D-455E-44FA-BCD8-395DA3499D2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18915" yWindow="3600" windowWidth="14400" windowHeight="7230" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTERNAL_LOADS" sheetId="1" r:id="rId1"/>
@@ -1518,7 +1518,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1566,7 +1566,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4">
         <v>21</v>
@@ -1592,7 +1592,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4">
         <v>21</v>
@@ -1619,7 +1619,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="4">
         <v>21</v>
@@ -1646,7 +1646,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="4">
         <v>21</v>
@@ -1673,7 +1673,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4">
         <v>21</v>
@@ -1700,7 +1700,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4">
         <v>20</v>
@@ -1727,7 +1727,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="4">
         <v>20</v>
@@ -1754,7 +1754,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="4">
         <v>21</v>
@@ -1781,7 +1781,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4">
         <v>18</v>
@@ -1808,7 +1808,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="4">
         <v>21</v>
@@ -1862,7 +1862,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="4">
         <v>18</v>
@@ -1889,7 +1889,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="4">
         <v>24</v>
@@ -1916,7 +1916,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="4">
         <v>18</v>
@@ -1942,7 +1942,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="4">
         <v>18</v>
@@ -1994,7 +1994,7 @@
         <v>30</v>
       </c>
       <c r="B18" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4">
         <v>21</v>
@@ -2021,7 +2021,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="4">
         <v>21</v>
@@ -2048,7 +2048,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="4">
         <v>21</v>
@@ -2075,7 +2075,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="4">
         <v>21</v>

</xml_diff>